<commit_message>
got cakes to work w/ second nav
</commit_message>
<xml_diff>
--- a/public/pricing.xlsx
+++ b/public/pricing.xlsx
@@ -90,18 +90,12 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,12 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -412,23 +403,26 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -451,12 +445,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -479,17 +473,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -540,12 +534,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -555,7 +549,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>